<commit_message>
add screen capture flag
</commit_message>
<xml_diff>
--- a/test_cases/e2e_test_cases.xlsx
+++ b/test_cases/e2e_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9144" tabRatio="500"/>
+    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="84">
   <si>
     <t>Case ID</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Actions</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
   </si>
   <si>
     <t>open_url</t>
@@ -277,10 +280,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -337,13 +340,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -358,8 +354,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -373,14 +385,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -411,6 +415,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -435,27 +446,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -465,15 +455,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,25 +505,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,49 +655,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,25 +673,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,73 +685,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,6 +710,21 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -753,23 +771,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -791,15 +803,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -811,7 +814,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -819,134 +822,134 @@
     <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -984,6 +987,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1373,17 +1382,17 @@
   <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.99074074074074" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="8.28703703703704" style="14" customWidth="1"/>
+    <col min="1" max="1" width="8.28571428571429" style="14" customWidth="1"/>
     <col min="2" max="2" width="33" style="14" customWidth="1"/>
-    <col min="3" max="3" width="33.7222222222222" style="14" customWidth="1"/>
+    <col min="3" max="3" width="33.7238095238095" style="14" customWidth="1"/>
     <col min="4" max="4" width="9" style="14"/>
-    <col min="5" max="5" width="5.57407407407407" style="14" customWidth="1"/>
+    <col min="5" max="5" width="5.57142857142857" style="14" customWidth="1"/>
     <col min="6" max="1024" width="9" style="14"/>
   </cols>
   <sheetData>
@@ -1438,7 +1447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="16.8" spans="1:5">
+    <row r="4" ht="15.75" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1471,12 +1480,12 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.99074074074074" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="8" style="14" customWidth="1"/>
-    <col min="2" max="2" width="7.86111111111111" style="14" customWidth="1"/>
-    <col min="3" max="3" width="11.7222222222222" style="14" customWidth="1"/>
-    <col min="4" max="4" width="19.4259259259259" style="14" customWidth="1"/>
+    <col min="2" max="2" width="7.85714285714286" style="14" customWidth="1"/>
+    <col min="3" max="3" width="11.7238095238095" style="14" customWidth="1"/>
+    <col min="4" max="4" width="19.4285714285714" style="14" customWidth="1"/>
     <col min="5" max="5" width="34" style="14" customWidth="1"/>
     <col min="6" max="1024" width="9" style="14"/>
   </cols>
@@ -1559,23 +1568,24 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.99074074074074" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="11.7222222222222" style="14" customWidth="1"/>
-    <col min="2" max="2" width="24.1388888888889" style="14" customWidth="1"/>
-    <col min="3" max="3" width="15.2777777777778" style="14" customWidth="1"/>
+    <col min="1" max="1" width="11.7238095238095" style="14" customWidth="1"/>
+    <col min="2" max="2" width="24.1428571428571" style="14" customWidth="1"/>
+    <col min="3" max="3" width="15.2761904761905" style="14" customWidth="1"/>
     <col min="4" max="4" width="32" style="14" customWidth="1"/>
-    <col min="5" max="5" width="17.4259259259259" style="14" customWidth="1"/>
-    <col min="6" max="1024" width="9" style="14"/>
+    <col min="5" max="5" width="17" style="15" customWidth="1"/>
+    <col min="6" max="6" width="11.2857142857143" style="15" customWidth="1"/>
+    <col min="7" max="1024" width="9" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:5">
+    <row r="1" ht="15.75" customHeight="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1591,8 +1601,11 @@
       <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:5">
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1601,13 +1614,14 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:5">
+      <c r="E2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1615,14 +1629,15 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:5">
+        <v>27</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -1630,16 +1645,17 @@
         <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:5">
+      <c r="E4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1647,14 +1663,15 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1" spans="1:5">
+        <v>27</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1662,14 +1679,17 @@
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:5">
+        <v>31</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1" spans="1:6">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1678,9 +1698,10 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1698,11 +1719,11 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.98148148148148" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.98095238095238" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="11.7314814814815" customWidth="1"/>
-    <col min="2" max="2" width="14.8611111111111" customWidth="1"/>
-    <col min="3" max="3" width="13.1388888888889" customWidth="1"/>
+    <col min="1" max="1" width="11.7333333333333" customWidth="1"/>
+    <col min="2" max="2" width="14.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="13.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1714,10 +1735,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4">
@@ -1725,13 +1746,13 @@
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4">
@@ -1739,13 +1760,13 @@
         <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1764,11 +1785,11 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.98148148148148" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.98095238095238" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="8.28703703703704" customWidth="1"/>
+    <col min="1" max="2" width="8.28571428571429" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="23.7314814814815" customWidth="1"/>
+    <col min="4" max="4" width="23.7333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:4">
@@ -1776,13 +1797,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4">
@@ -1793,10 +1814,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4">
@@ -1807,10 +1828,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:4">
@@ -1821,10 +1842,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:4">
@@ -1835,10 +1856,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:4">
@@ -1849,10 +1870,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:4">
@@ -1863,10 +1884,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1889,32 +1910,32 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.41666666666667" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1388888888889" style="1" customWidth="1"/>
-    <col min="2" max="3" width="21.2777777777778" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7314814814815" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1428571428571" style="1" customWidth="1"/>
+    <col min="2" max="3" width="21.2761904761905" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7333333333333" style="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.71296296296296" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2222222222222" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.2685185185185" style="1" customWidth="1"/>
-    <col min="9" max="9" width="38.2685185185185" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.71428571428571" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2190476190476" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.2666666666667" style="1" customWidth="1"/>
+    <col min="9" max="9" width="38.2666666666667" style="1" customWidth="1"/>
     <col min="10" max="10" width="5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.57407407407407" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5833333333333" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.57142857142857" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5809523809524" style="1" customWidth="1"/>
     <col min="13" max="13" width="28" style="1" customWidth="1"/>
-    <col min="14" max="14" width="26.8796296296296" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.4259259259259" style="1" customWidth="1"/>
-    <col min="16" max="16" width="34.9722222222222" style="1" customWidth="1"/>
-    <col min="17" max="17" width="6.86111111111111" style="1" customWidth="1"/>
-    <col min="18" max="18" width="30.8703703703704" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.1388888888889" style="1" customWidth="1"/>
-    <col min="20" max="1024" width="9.42592592592593" style="1"/>
+    <col min="14" max="14" width="26.8761904761905" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.4285714285714" style="1" customWidth="1"/>
+    <col min="16" max="16" width="34.9714285714286" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.85714285714286" style="1" customWidth="1"/>
+    <col min="18" max="18" width="30.8666666666667" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1428571428571" style="1" customWidth="1"/>
+    <col min="20" max="1024" width="9.42857142857143" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:19">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1923,22 +1944,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
@@ -1947,48 +1968,48 @@
         <v>4</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" ht="16.5" customHeight="1" spans="1:19">
       <c r="A2" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
       <c r="J2" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3">
@@ -2004,32 +2025,32 @@
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:19">
       <c r="A3" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="4"/>
       <c r="J3" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3">
         <v>200</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
@@ -2048,22 +2069,22 @@
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>7</v>
@@ -2075,10 +2096,10 @@
         <v>200</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="6"/>
@@ -2091,28 +2112,28 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>7</v>
@@ -2124,10 +2145,10 @@
         <v>200</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="6"/>
@@ -2147,19 +2168,19 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>7</v>
@@ -2171,10 +2192,10 @@
         <v>200</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="4"/>
@@ -2182,7 +2203,7 @@
       <c r="R6" s="6"/>
       <c r="S6" s="10"/>
     </row>
-    <row r="9" ht="15" customHeight="1" spans="17:17">
+    <row r="9" customHeight="1" spans="17:17">
       <c r="Q9" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support using variable in ui test
</commit_message>
<xml_diff>
--- a/test_cases/e2e_test_cases.xlsx
+++ b/test_cases/e2e_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="500"/>
+    <workbookView windowWidth="23040" windowHeight="9144" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="79">
   <si>
     <t>Case ID</t>
   </si>
@@ -37,16 +37,25 @@
     <t>Tags</t>
   </si>
   <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>pacs008 in cny 100</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>tag1</t>
+  </si>
+  <si>
     <t>TC001</t>
   </si>
   <si>
     <t>Search for software testing</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>tag1</t>
+    <t>n</t>
   </si>
   <si>
     <t>TC002</t>
@@ -55,12 +64,6 @@
     <t>Search for frontend development</t>
   </si>
   <si>
-    <t>TC003</t>
-  </si>
-  <si>
-    <t>pacs008 in cny 100</t>
-  </si>
-  <si>
     <t>Step ID</t>
   </si>
   <si>
@@ -151,7 +154,7 @@
     <t>TC001性能测试</t>
   </si>
   <si>
-    <t>TC002自动化测试</t>
+    <t>TC002自动化测试 ${TC002.$.result.amount}</t>
   </si>
   <si>
     <t>TCID</t>
@@ -264,9 +267,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -300,16 +303,98 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -321,29 +406,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,71 +427,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -432,28 +451,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -470,31 +473,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,7 +611,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,139 +653,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -679,26 +682,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -744,11 +732,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -770,16 +771,18 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -787,130 +790,130 @@
     <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1329,16 +1332,16 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.99074074074074" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="8.28571428571429" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.28703703703704" style="7" customWidth="1"/>
     <col min="2" max="2" width="33" style="7" customWidth="1"/>
-    <col min="3" max="3" width="33.7238095238095" style="7" customWidth="1"/>
+    <col min="3" max="3" width="33.7222222222222" style="7" customWidth="1"/>
     <col min="4" max="4" width="9" style="7"/>
-    <col min="5" max="5" width="5.57142857142857" style="7" customWidth="1"/>
+    <col min="5" max="5" width="5.57407407407407" style="7" customWidth="1"/>
     <col min="6" max="1024" width="9" style="7"/>
   </cols>
   <sheetData>
@@ -1359,7 +1362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:5">
+    <row r="2" ht="16.8" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1387,21 +1390,21 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="1:5">
+    <row r="4" ht="15.75" customHeight="1" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
@@ -1426,12 +1429,12 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.99074074074074" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="8" style="7" customWidth="1"/>
-    <col min="2" max="2" width="7.85714285714286" style="7" customWidth="1"/>
-    <col min="3" max="3" width="11.7238095238095" style="7" customWidth="1"/>
-    <col min="4" max="4" width="19.4285714285714" style="7" customWidth="1"/>
+    <col min="2" max="2" width="7.86111111111111" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11.7222222222222" style="7" customWidth="1"/>
+    <col min="4" max="4" width="19.4259259259259" style="7" customWidth="1"/>
     <col min="5" max="5" width="34" style="7" customWidth="1"/>
     <col min="6" max="1024" width="9" style="7"/>
   </cols>
@@ -1441,67 +1444,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1520,115 +1523,115 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.99074074074074" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="11.7238095238095" style="7" customWidth="1"/>
-    <col min="2" max="2" width="24.1428571428571" style="7" customWidth="1"/>
-    <col min="3" max="3" width="15.2761904761905" style="7" customWidth="1"/>
+    <col min="1" max="1" width="11.7222222222222" style="7" customWidth="1"/>
+    <col min="2" max="2" width="24.1388888888889" style="7" customWidth="1"/>
+    <col min="3" max="3" width="15.2777777777778" style="7" customWidth="1"/>
     <col min="4" max="4" width="32" style="7" customWidth="1"/>
     <col min="5" max="5" width="17" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.2857142857143" style="8" customWidth="1"/>
+    <col min="6" max="6" width="11.287037037037" style="8" customWidth="1"/>
     <col min="7" max="1024" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="9"/>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
@@ -1651,54 +1654,54 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.98095238095238" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.98148148148148" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="11.7333333333333" customWidth="1"/>
-    <col min="2" max="2" width="14.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="13.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="11.7314814814815" customWidth="1"/>
+    <col min="2" max="2" width="14.8611111111111" customWidth="1"/>
+    <col min="3" max="3" width="13.1388888888889" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1714,14 +1717,14 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.98095238095238" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.98148148148148" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="8.28571428571429" customWidth="1"/>
+    <col min="1" max="2" width="8.28703703703704" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="23.7333333333333" customWidth="1"/>
+    <col min="4" max="4" width="23.7314814814815" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:4">
@@ -1729,97 +1732,97 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1838,32 +1841,32 @@
   <sheetPr/>
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.41666666666667" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.1428571428571" style="1" customWidth="1"/>
-    <col min="2" max="3" width="21.2761904761905" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7333333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1388888888889" style="1" customWidth="1"/>
+    <col min="2" max="3" width="21.2777777777778" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7314814814815" style="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.71428571428571" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.2190476190476" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.2666666666667" style="1" customWidth="1"/>
-    <col min="9" max="9" width="38.2666666666667" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.71296296296296" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2222222222222" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.2685185185185" style="1" customWidth="1"/>
+    <col min="9" max="9" width="38.2685185185185" style="1" customWidth="1"/>
     <col min="10" max="10" width="5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.57142857142857" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5809523809524" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.57407407407407" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5833333333333" style="1" customWidth="1"/>
     <col min="13" max="13" width="28" style="1" customWidth="1"/>
-    <col min="14" max="14" width="26.8761904761905" style="1" customWidth="1"/>
-    <col min="15" max="1019" width="9.42857142857143" style="1"/>
-    <col min="1020" max="1020" width="9.42857142857143"/>
+    <col min="14" max="14" width="26.8796296296296" style="1" customWidth="1"/>
+    <col min="15" max="1019" width="9.42592592592593" style="1"/>
+    <col min="1020" max="1020" width="9.42592592592593"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:14">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1872,22 +1875,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
@@ -1896,100 +1899,100 @@
         <v>4</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" ht="16.5" customHeight="1" spans="1:14">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
       <c r="J2" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3">
         <v>200</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:14">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="4"/>
       <c r="J3" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3">
         <v>200</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" ht="31.5" spans="1:14">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" ht="33.6" spans="1:14">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>7</v>
@@ -2001,39 +2004,39 @@
         <v>200</v>
       </c>
       <c r="M4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" ht="16.8" spans="1:14">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" spans="1:14">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>7</v>
@@ -2045,39 +2048,39 @@
         <v>200</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" ht="31.5" spans="1:14">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" ht="33.6" spans="1:14">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>7</v>
@@ -2089,13 +2092,13 @@
         <v>200</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" customHeight="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
add table verify and wait
</commit_message>
<xml_diff>
--- a/test_cases/e2e_test_cases.xlsx
+++ b/test_cases/e2e_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="653" activeTab="4"/>
+    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="653" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="126">
   <si>
     <t>Case ID</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Screenshot</t>
+  </si>
+  <si>
+    <t>Wait</t>
   </si>
   <si>
     <t>open_url</t>
@@ -531,10 +534,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -574,6 +577,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -589,7 +599,31 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -603,9 +637,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -635,7 +668,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -650,23 +698,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -675,35 +707,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -737,13 +740,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,91 +884,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,73 +914,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -942,6 +945,26 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1000,6 +1023,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1014,39 +1046,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1057,127 +1060,127 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1755,23 +1758,23 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="1" ht="201" customHeight="1" spans="1:2">
       <c r="A2" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" s="6" customFormat="1" ht="201" customHeight="1" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1805,92 +1808,92 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.75" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="90" spans="1:10">
       <c r="A2" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C2" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="90" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1909,7 +1912,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -2000,13 +2003,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="11.7238095238095" style="16" customWidth="1"/>
     <col min="2" max="2" width="24.1428571428571" style="16" customWidth="1"/>
@@ -2017,7 +2020,7 @@
     <col min="7" max="1024" width="9" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:6">
+    <row r="1" ht="15.75" customHeight="1" spans="1:7">
       <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
@@ -2036,8 +2039,11 @@
       <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:6">
+    <row r="2" ht="15.75" customHeight="1" spans="1:7">
       <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
@@ -2046,14 +2052,15 @@
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:6">
+    <row r="3" ht="15.75" customHeight="1" spans="1:7">
       <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
@@ -2061,15 +2068,16 @@
         <v>18</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:6">
+    <row r="4" ht="15.75" customHeight="1" spans="1:7">
       <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
@@ -2077,17 +2085,18 @@
         <v>18</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:6">
+    <row r="5" ht="15.75" customHeight="1" spans="1:7">
       <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
@@ -2095,15 +2104,16 @@
         <v>18</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1" spans="1:6">
+    <row r="6" ht="15.75" customHeight="1" spans="1:7">
       <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
@@ -2111,17 +2121,18 @@
         <v>18</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="18" t="s">
         <v>7</v>
       </c>
+      <c r="G6" s="18"/>
     </row>
-    <row r="7" ht="15.75" spans="1:6">
+    <row r="7" ht="15.75" spans="1:7">
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
@@ -2130,12 +2141,13 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2155,7 +2167,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.98095238095238" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
@@ -2174,10 +2186,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4">
@@ -2185,13 +2197,13 @@
         <v>17</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4">
@@ -2199,13 +2211,13 @@
         <v>17</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2220,7 +2232,7 @@
   <sheetPr/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:D10"/>
     </sheetView>
   </sheetViews>
@@ -2236,13 +2248,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4">
@@ -2253,10 +2265,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4">
@@ -2267,10 +2279,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:4">
@@ -2281,10 +2293,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:4">
@@ -2295,10 +2307,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:4">
@@ -2309,10 +2321,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:4">
@@ -2323,10 +2335,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:4">
@@ -2337,10 +2349,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:4">
@@ -2351,10 +2363,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="1:4">
@@ -2365,10 +2377,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2413,7 +2425,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:14">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2422,22 +2434,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
@@ -2446,75 +2458,75 @@
         <v>4</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" ht="16.5" customHeight="1" spans="1:14">
       <c r="A2" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="11"/>
       <c r="J2" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K2" s="10"/>
       <c r="L2" s="10">
         <v>200</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N2" s="11"/>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:14">
       <c r="A3" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="11"/>
       <c r="J3" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K3" s="10"/>
       <c r="L3" s="10">
         <v>200</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" ht="31.5" customHeight="1" spans="1:14">
@@ -2528,22 +2540,22 @@
         <v>6</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>7</v>
@@ -2555,10 +2567,10 @@
         <v>200</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:14">
@@ -2566,28 +2578,28 @@
         <v>11</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>7</v>
@@ -2599,10 +2611,10 @@
         <v>200</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" ht="47.25" spans="1:14">
@@ -2616,22 +2628,22 @@
         <v>6</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>7</v>
@@ -2643,10 +2655,10 @@
         <v>200</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" s="6" customFormat="1" spans="1:1019">
@@ -5739,142 +5751,142 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" ht="15.75" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="1" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" s="6" customFormat="1" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" s="6" customFormat="1" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" s="6" customFormat="1" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" s="6" customFormat="1" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" s="6" customFormat="1" spans="1:4">
       <c r="A7" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" s="6" customFormat="1" spans="1:4">
       <c r="A8" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" s="6" customFormat="1" spans="1:4">
       <c r="A9" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" s="6" customFormat="1" spans="1:4">
       <c r="A10" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -5912,26 +5924,26 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" ht="15.75" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="1" ht="105" spans="1:2">
       <c r="A2" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" s="6" customFormat="1" ht="60" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -5958,35 +5970,35 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" ht="15.75" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="1" ht="201" customHeight="1" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" s="6" customFormat="1" ht="201" customHeight="1" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data type in the data sheet
</commit_message>
<xml_diff>
--- a/test_cases/e2e_test_cases.xlsx
+++ b/test_cases/e2e_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="653" activeTab="2"/>
+    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="653" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="127">
   <si>
     <t>Case ID</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Data Set</t>
+  </si>
+  <si>
+    <t>Data Type</t>
   </si>
   <si>
     <t>Value</t>
@@ -534,8 +537,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -558,6 +561,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -568,11 +578,6 @@
     <font>
       <sz val="10.5"/>
       <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -590,6 +595,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -598,10 +610,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -613,17 +631,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -645,8 +654,46 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -661,29 +708,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -692,28 +717,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -740,19 +743,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,7 +767,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -782,19 +791,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -812,37 +821,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -854,25 +863,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -890,7 +881,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -902,25 +923,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -949,26 +952,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -980,30 +963,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1025,9 +984,53 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1049,142 +1052,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1217,13 +1220,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1654,12 +1661,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="8.28571428571429" style="16" customWidth="1"/>
-    <col min="2" max="2" width="33" style="16" customWidth="1"/>
-    <col min="3" max="3" width="33.7238095238095" style="16" customWidth="1"/>
-    <col min="4" max="4" width="9" style="16"/>
-    <col min="5" max="5" width="5.57142857142857" style="16" customWidth="1"/>
-    <col min="6" max="1024" width="9" style="16"/>
+    <col min="1" max="1" width="8.28571428571429" style="18" customWidth="1"/>
+    <col min="2" max="2" width="33" style="18" customWidth="1"/>
+    <col min="3" max="3" width="33.7238095238095" style="18" customWidth="1"/>
+    <col min="4" max="4" width="9" style="18"/>
+    <col min="5" max="5" width="5.57142857142857" style="18" customWidth="1"/>
+    <col min="6" max="1024" width="9" style="18"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:5">
@@ -1680,53 +1687,53 @@
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:5">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1758,23 +1765,23 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="1" ht="201" customHeight="1" spans="1:2">
       <c r="A2" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" s="6" customFormat="1" ht="201" customHeight="1" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1808,92 +1815,92 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.75" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="90" spans="1:10">
       <c r="A2" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C2" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="90" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1917,12 +1924,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="8" style="16" customWidth="1"/>
-    <col min="2" max="2" width="7.85714285714286" style="16" customWidth="1"/>
-    <col min="3" max="3" width="11.7238095238095" style="16" customWidth="1"/>
-    <col min="4" max="4" width="19.4285714285714" style="16" customWidth="1"/>
-    <col min="5" max="5" width="34" style="16" customWidth="1"/>
-    <col min="6" max="1024" width="9" style="16"/>
+    <col min="1" max="1" width="8" style="18" customWidth="1"/>
+    <col min="2" max="2" width="7.85714285714286" style="18" customWidth="1"/>
+    <col min="3" max="3" width="11.7238095238095" style="18" customWidth="1"/>
+    <col min="4" max="4" width="19.4285714285714" style="18" customWidth="1"/>
+    <col min="5" max="5" width="34" style="18" customWidth="1"/>
+    <col min="6" max="1024" width="9" style="18"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:5">
@@ -1943,53 +1950,53 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="17">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="17">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:5">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="17">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="17" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2005,35 +2012,35 @@
   <sheetPr/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="11.7238095238095" style="16" customWidth="1"/>
-    <col min="2" max="2" width="24.1428571428571" style="16" customWidth="1"/>
-    <col min="3" max="3" width="15.2761904761905" style="16" customWidth="1"/>
-    <col min="4" max="4" width="32" style="16" customWidth="1"/>
-    <col min="5" max="5" width="17" style="17" customWidth="1"/>
-    <col min="6" max="6" width="11.2857142857143" style="17" customWidth="1"/>
-    <col min="7" max="1024" width="9" style="16"/>
+    <col min="1" max="1" width="11.7238095238095" style="18" customWidth="1"/>
+    <col min="2" max="2" width="24.1428571428571" style="18" customWidth="1"/>
+    <col min="3" max="3" width="15.2761904761905" style="18" customWidth="1"/>
+    <col min="4" max="4" width="32" style="18" customWidth="1"/>
+    <col min="5" max="5" width="17" style="19" customWidth="1"/>
+    <col min="6" max="6" width="11.2857142857143" style="19" customWidth="1"/>
+    <col min="7" max="1024" width="9" style="18"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:7">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -2057,8 +2064,8 @@
       <c r="E2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:7">
       <c r="A3" s="10" t="s">
@@ -2074,8 +2081,8 @@
         <v>28</v>
       </c>
       <c r="E3" s="10"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:7">
       <c r="A4" s="10" t="s">
@@ -2093,8 +2100,8 @@
       <c r="E4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:7">
       <c r="A5" s="10" t="s">
@@ -2110,8 +2117,8 @@
         <v>28</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:7">
       <c r="A6" s="10" t="s">
@@ -2127,10 +2134,10 @@
         <v>32</v>
       </c>
       <c r="E6" s="10"/>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" ht="15.75" spans="1:7">
       <c r="A7" s="10" t="s">
@@ -2146,8 +2153,8 @@
       <c r="E7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2193,30 +2200,30 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="17" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="17" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2230,34 +2237,38 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.98095238095238" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.98095238095238" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="2" width="8.28571428571429" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="23.7333333333333" customWidth="1"/>
+    <col min="4" max="4" width="10.4285714285714" style="12" customWidth="1"/>
+    <col min="5" max="5" width="23.7333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+    <row r="1" ht="15.75" customHeight="1" spans="1:5">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>42</v>
       </c>
+      <c r="E1" s="13" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:4">
+    <row r="2" ht="15.75" customHeight="1" spans="1:5">
       <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
@@ -2267,11 +2278,12 @@
       <c r="C2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>43</v>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:4">
+    <row r="3" ht="15.75" customHeight="1" spans="1:5">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2281,11 +2293,12 @@
       <c r="C3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>44</v>
+      <c r="D3" s="14"/>
+      <c r="E3" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:4">
+    <row r="4" ht="15.75" customHeight="1" spans="1:5">
       <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
@@ -2295,11 +2308,12 @@
       <c r="C4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>45</v>
+      <c r="D4" s="14"/>
+      <c r="E4" s="16" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:4">
+    <row r="5" ht="15.75" customHeight="1" spans="1:5">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -2309,11 +2323,12 @@
       <c r="C5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>43</v>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1" spans="1:4">
+    <row r="6" ht="15.75" customHeight="1" spans="1:5">
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
@@ -2323,11 +2338,12 @@
       <c r="C6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>46</v>
+      <c r="D6" s="14"/>
+      <c r="E6" s="16" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:4">
+    <row r="7" ht="15.75" customHeight="1" spans="1:5">
       <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
@@ -2337,11 +2353,12 @@
       <c r="C7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>45</v>
+      <c r="D7" s="14"/>
+      <c r="E7" s="16" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="1:4">
+    <row r="8" ht="15.75" spans="1:5">
       <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
@@ -2351,11 +2368,12 @@
       <c r="C8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>43</v>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="9" ht="15.75" spans="1:4">
+    <row r="9" ht="15.75" spans="1:5">
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
@@ -2365,11 +2383,12 @@
       <c r="C9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>47</v>
+      <c r="D9" s="14"/>
+      <c r="E9" s="16" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="10" ht="15.75" spans="1:4">
+    <row r="10" ht="15.75" spans="1:5">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -2379,14 +2398,15 @@
       <c r="C10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>45</v>
+      <c r="D10" s="14"/>
+      <c r="E10" s="16" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="http://www.baidu.com" tooltip="http://www.baidu.com"/>
-    <hyperlink ref="D5" r:id="rId1" display="http://www.baidu.com" tooltip="http://www.baidu.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="http://www.baidu.com" tooltip="http://www.baidu.com"/>
+    <hyperlink ref="E5" r:id="rId1" display="http://www.baidu.com" tooltip="http://www.baidu.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2425,7 +2445,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:14">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2434,22 +2454,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
@@ -2458,75 +2478,75 @@
         <v>4</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" ht="16.5" customHeight="1" spans="1:14">
       <c r="A2" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="11"/>
       <c r="J2" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K2" s="10"/>
       <c r="L2" s="10">
         <v>200</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N2" s="11"/>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:14">
       <c r="A3" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="11"/>
       <c r="J3" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K3" s="10"/>
       <c r="L3" s="10">
         <v>200</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" ht="31.5" customHeight="1" spans="1:14">
@@ -2540,22 +2560,22 @@
         <v>6</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>7</v>
@@ -2567,10 +2587,10 @@
         <v>200</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:14">
@@ -2578,28 +2598,28 @@
         <v>11</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>7</v>
@@ -2611,10 +2631,10 @@
         <v>200</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" ht="47.25" spans="1:14">
@@ -2628,22 +2648,22 @@
         <v>6</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>7</v>
@@ -2655,10 +2675,10 @@
         <v>200</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" s="6" customFormat="1" spans="1:1019">
@@ -5751,142 +5771,142 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" ht="15.75" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="1" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" s="6" customFormat="1" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" s="6" customFormat="1" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" s="6" customFormat="1" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" s="6" customFormat="1" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" s="6" customFormat="1" spans="1:4">
       <c r="A7" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" s="6" customFormat="1" spans="1:4">
       <c r="A8" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" s="6" customFormat="1" spans="1:4">
       <c r="A9" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" s="6" customFormat="1" spans="1:4">
       <c r="A10" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -5924,26 +5944,26 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" ht="15.75" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="1" ht="105" spans="1:2">
       <c r="A2" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" s="6" customFormat="1" ht="60" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -5970,35 +5990,35 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" ht="15.75" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="1" ht="201" customHeight="1" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" s="6" customFormat="1" ht="201" customHeight="1" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add webtest load validation
</commit_message>
<xml_diff>
--- a/test_cases/e2e_test_cases.xlsx
+++ b/test_cases/e2e_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="653" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9144" tabRatio="653" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="128">
   <si>
     <t>Case ID</t>
   </si>
@@ -547,10 +547,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -591,39 +591,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -641,9 +611,107 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -658,75 +726,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -753,13 +753,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -771,7 +789,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -783,7 +801,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -795,109 +915,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -909,31 +933,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -962,20 +962,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -997,11 +994,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1021,17 +1031,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1045,155 +1049,151 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1663,16 +1663,16 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D$1:D$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.99074074074074" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="8.28571428571429" style="17" customWidth="1"/>
+    <col min="1" max="1" width="8.28703703703704" style="17" customWidth="1"/>
     <col min="2" max="2" width="33" style="17" customWidth="1"/>
-    <col min="3" max="3" width="33.7238095238095" style="17" customWidth="1"/>
+    <col min="3" max="3" width="33.7222222222222" style="17" customWidth="1"/>
     <col min="4" max="4" width="9" style="17"/>
-    <col min="5" max="5" width="5.57142857142857" style="17" customWidth="1"/>
+    <col min="5" max="5" width="5.57407407407407" style="17" customWidth="1"/>
     <col min="6" max="1024" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -1693,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:5">
+    <row r="2" ht="16.8" spans="1:5">
       <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
@@ -1760,14 +1760,14 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="17.552380952381" style="6" customWidth="1"/>
-    <col min="2" max="2" width="118.780952380952" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="9.14285714285714" style="6"/>
+    <col min="1" max="1" width="17.5555555555556" style="6" customWidth="1"/>
+    <col min="2" max="2" width="118.777777777778" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="9.13888888888889" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="15.75" spans="1:2">
+    <row r="1" s="6" customFormat="1" ht="16.8" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1806,21 +1806,21 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.11428571428571" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="13.1142857142857" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1111111111111" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.66666666666667" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.447619047619" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.4444444444444" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.3333333333333" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.552380952381" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.552380952381" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5555555555556" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5555555555556" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.6666666666667" style="1" customWidth="1"/>
-    <col min="9" max="9" width="48.552380952381" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.11428571428571" style="1" customWidth="1"/>
+    <col min="9" max="9" width="48.5555555555556" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.11111111111111" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="15.75" spans="1:9">
+    <row r="1" s="1" customFormat="1" ht="16.8" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="105" spans="1:10">
+    <row r="2" s="1" customFormat="1" ht="100.8" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>85</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="105" spans="1:9">
+    <row r="3" s="1" customFormat="1" ht="100.8" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>91</v>
       </c>
@@ -1923,23 +1923,23 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="F1" sqref="F$1:F$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.99074074074074" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="8" style="17" customWidth="1"/>
-    <col min="2" max="2" width="7.85714285714286" style="17" customWidth="1"/>
-    <col min="3" max="3" width="11.7238095238095" style="17" customWidth="1"/>
-    <col min="4" max="4" width="19.4285714285714" style="17" customWidth="1"/>
+    <col min="2" max="2" width="7.86111111111111" style="17" customWidth="1"/>
+    <col min="3" max="3" width="11.7222222222222" style="17" customWidth="1"/>
+    <col min="4" max="4" width="19.4259259259259" style="17" customWidth="1"/>
     <col min="5" max="5" width="34" style="17" customWidth="1"/>
     <col min="6" max="1024" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:5">
+    <row r="1" ht="15.75" customHeight="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1955,8 +1955,11 @@
       <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:5">
+    <row r="2" ht="15.75" customHeight="1" spans="1:6">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
@@ -1972,8 +1975,11 @@
       <c r="E2" s="16" t="s">
         <v>19</v>
       </c>
+      <c r="F2" s="16" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:5">
+    <row r="3" ht="15.75" customHeight="1" spans="1:6">
       <c r="A3" s="16" t="s">
         <v>11</v>
       </c>
@@ -1989,8 +1995,11 @@
       <c r="E3" s="16" t="s">
         <v>19</v>
       </c>
+      <c r="F3" s="16" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:5">
+    <row r="4" ht="15.75" customHeight="1" spans="1:6">
       <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
@@ -2005,6 +2014,9 @@
       </c>
       <c r="E4" s="16" t="s">
         <v>11</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2017,25 +2029,25 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F$1:H$1048576"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.99074074074074" defaultRowHeight="14.4" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="11.7238095238095" style="17" customWidth="1"/>
-    <col min="2" max="2" width="24.1428571428571" style="17" customWidth="1"/>
-    <col min="3" max="3" width="15.2761904761905" style="17" customWidth="1"/>
+    <col min="1" max="1" width="11.7222222222222" style="17" customWidth="1"/>
+    <col min="2" max="2" width="24.1388888888889" style="17" customWidth="1"/>
+    <col min="3" max="3" width="15.2777777777778" style="17" customWidth="1"/>
     <col min="4" max="4" width="32" style="17" customWidth="1"/>
     <col min="5" max="5" width="17" style="18" customWidth="1"/>
-    <col min="6" max="6" width="9.28571428571429" style="18" customWidth="1"/>
-    <col min="7" max="7" width="11.2857142857143" style="18" customWidth="1"/>
+    <col min="6" max="6" width="9.28703703703704" style="18" customWidth="1"/>
+    <col min="7" max="7" width="11.287037037037" style="18" customWidth="1"/>
     <col min="8" max="1025" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:8">
+    <row r="1" ht="15.75" customHeight="1" spans="1:9">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -2060,8 +2072,11 @@
       <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:8">
+    <row r="2" ht="15.75" customHeight="1" spans="1:9">
       <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
@@ -2078,8 +2093,11 @@
       <c r="F2" s="10"/>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
+      <c r="I2" s="16" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:8">
+    <row r="3" ht="15.75" customHeight="1" spans="1:9">
       <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
@@ -2100,8 +2118,11 @@
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
+      <c r="I3" s="16" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:8">
+    <row r="4" ht="15.75" customHeight="1" spans="1:9">
       <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
@@ -2122,8 +2143,11 @@
         <v>7</v>
       </c>
       <c r="H4" s="19"/>
+      <c r="I4" s="16" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" ht="15.75" spans="1:8">
+    <row r="5" ht="16.8" spans="1:9">
       <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
@@ -2141,6 +2165,9 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19">
         <v>1</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2164,11 +2191,11 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.98095238095238" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.98148148148148" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="11.7333333333333" customWidth="1"/>
-    <col min="2" max="2" width="14.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="13.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="11.7314814814815" customWidth="1"/>
+    <col min="2" max="2" width="14.8611111111111" customWidth="1"/>
+    <col min="3" max="3" width="13.1388888888889" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2230,12 +2257,12 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.98095238095238" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.98148148148148" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="2" width="8.28571428571429" customWidth="1"/>
+    <col min="1" max="2" width="8.28703703703704" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="10.4285714285714" style="12" customWidth="1"/>
-    <col min="5" max="5" width="23.7333333333333" customWidth="1"/>
+    <col min="4" max="4" width="10.4259259259259" style="12" customWidth="1"/>
+    <col min="5" max="5" width="23.7314814814815" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:5">
@@ -2345,7 +2372,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="1:5">
+    <row r="8" ht="16.8" spans="1:5">
       <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
@@ -2360,7 +2387,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" ht="15.75" spans="1:5">
+    <row r="9" ht="16.8" spans="1:5">
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
@@ -2375,7 +2402,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" ht="15.75" spans="1:5">
+    <row r="10" ht="16.8" spans="1:5">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -2410,24 +2437,24 @@
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.41666666666667" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.1428571428571" style="9" customWidth="1"/>
-    <col min="2" max="3" width="21.2857142857143" style="9" customWidth="1"/>
-    <col min="4" max="4" width="24.7333333333333" style="9" customWidth="1"/>
+    <col min="1" max="1" width="13.1388888888889" style="9" customWidth="1"/>
+    <col min="2" max="3" width="21.287037037037" style="9" customWidth="1"/>
+    <col min="4" max="4" width="24.7314814814815" style="9" customWidth="1"/>
     <col min="5" max="5" width="20" style="9" customWidth="1"/>
-    <col min="6" max="6" width="8.71428571428571" style="9" customWidth="1"/>
-    <col min="7" max="7" width="17.2190476190476" style="9" customWidth="1"/>
-    <col min="8" max="8" width="18.2761904761905" style="9" customWidth="1"/>
-    <col min="9" max="9" width="38.2666666666667" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.71296296296296" style="9" customWidth="1"/>
+    <col min="7" max="7" width="17.2222222222222" style="9" customWidth="1"/>
+    <col min="8" max="8" width="18.2777777777778" style="9" customWidth="1"/>
+    <col min="9" max="9" width="38.2685185185185" style="9" customWidth="1"/>
     <col min="10" max="10" width="5" style="9" customWidth="1"/>
-    <col min="11" max="11" width="5.57142857142857" style="9" customWidth="1"/>
-    <col min="12" max="12" width="10.5809523809524" style="9" customWidth="1"/>
+    <col min="11" max="11" width="5.57407407407407" style="9" customWidth="1"/>
+    <col min="12" max="12" width="10.5833333333333" style="9" customWidth="1"/>
     <col min="13" max="13" width="28" style="9" customWidth="1"/>
-    <col min="14" max="14" width="26.8761904761905" style="9" customWidth="1"/>
-    <col min="15" max="1019" width="9.42857142857143" style="9"/>
-    <col min="1020" max="1020" width="9.42857142857143" style="6"/>
-    <col min="1021" max="16384" width="9.41904761904762" style="6"/>
+    <col min="14" max="14" width="26.8796296296296" style="9" customWidth="1"/>
+    <col min="15" max="1019" width="9.42592592592593" style="9"/>
+    <col min="1020" max="1020" width="9.42592592592593" style="6"/>
+    <col min="1021" max="16384" width="9.41666666666667" style="6"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:14">
@@ -2580,7 +2607,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" ht="15.75" spans="1:14">
+    <row r="5" ht="16.8" spans="1:14">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
@@ -2624,7 +2651,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" ht="47.25" spans="1:14">
+    <row r="6" ht="50.4" spans="1:14">
       <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
@@ -4710,7 +4737,7 @@
       <c r="AMD8" s="9"/>
       <c r="AME8" s="9"/>
     </row>
-    <row r="9" s="6" customFormat="1" customHeight="1" spans="1:1019">
+    <row r="9" s="6" customFormat="1" ht="15" customHeight="1" spans="1:1019">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -5747,16 +5774,16 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="17.552380952381" style="6" customWidth="1"/>
-    <col min="2" max="2" width="20.7809523809524" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17.552380952381" style="6" customWidth="1"/>
-    <col min="4" max="4" width="57.1142857142857" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.14285714285714" style="6"/>
+    <col min="1" max="1" width="17.5555555555556" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.7777777777778" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.5555555555556" style="6" customWidth="1"/>
+    <col min="4" max="4" width="57.1111111111111" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.13888888888889" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="15.75" spans="1:4">
+    <row r="1" s="6" customFormat="1" ht="16.8" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -5922,14 +5949,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="12.7809523809524" style="6" customWidth="1"/>
-    <col min="2" max="2" width="118.780952380952" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="9.14285714285714" style="6"/>
+    <col min="1" max="1" width="12.7777777777778" style="6" customWidth="1"/>
+    <col min="2" max="2" width="118.777777777778" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="9.13888888888889" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="15.75" spans="1:2">
+    <row r="1" s="6" customFormat="1" ht="16.8" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>99</v>
       </c>
@@ -5937,7 +5964,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" s="6" customFormat="1" ht="105" spans="1:2">
+    <row r="2" s="6" customFormat="1" ht="100.8" spans="1:2">
       <c r="A2" s="7" t="s">
         <v>61</v>
       </c>
@@ -5945,7 +5972,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" s="6" customFormat="1" ht="60" spans="1:2">
+    <row r="3" s="6" customFormat="1" ht="57.6" spans="1:2">
       <c r="A3" s="7" t="s">
         <v>75</v>
       </c>
@@ -5968,14 +5995,14 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="2" width="14.7809523809524" style="6" customWidth="1"/>
-    <col min="3" max="3" width="118.780952380952" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="9.14285714285714" style="6"/>
+    <col min="1" max="2" width="14.7777777777778" style="6" customWidth="1"/>
+    <col min="3" max="3" width="118.777777777778" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="9.13888888888889" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="15.75" spans="1:3">
+    <row r="1" s="6" customFormat="1" ht="16.8" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>103</v>
       </c>

</xml_diff>

<commit_message>
Optimize parameter excel input
</commit_message>
<xml_diff>
--- a/test_cases/e2e_test_cases.xlsx
+++ b/test_cases/e2e_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="850" activeTab="2"/>
+    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="850" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="139">
   <si>
     <t>Case ID</t>
   </si>
@@ -46,30 +46,30 @@
     <t>Tags</t>
   </si>
   <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>pacs008 in cny 100</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>tag1,sanity check</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>Search for software testing</t>
+  </si>
+  <si>
+    <t>tag1</t>
+  </si>
+  <si>
     <t>TC003</t>
   </si>
   <si>
-    <t>pacs008 in cny 100</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>tag1,sanity check</t>
-  </si>
-  <si>
-    <t>TC001</t>
-  </si>
-  <si>
-    <t>Search for software testing</t>
-  </si>
-  <si>
-    <t>tag1</t>
-  </si>
-  <si>
-    <t>TC002</t>
-  </si>
-  <si>
     <t>Search for frontend development</t>
   </si>
   <si>
@@ -82,27 +82,27 @@
     <t>Module Name</t>
   </si>
   <si>
+    <t>APIs</t>
+  </si>
+  <si>
+    <t>Baidu</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Element Name</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
     <t>Parameter Name</t>
   </si>
   <si>
-    <t>Baidu</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>url,search_term,expected_title</t>
-  </si>
-  <si>
-    <t>API</t>
-  </si>
-  <si>
-    <t>Element Name</t>
-  </si>
-  <si>
-    <t>Actions</t>
-  </si>
-  <si>
     <t>Highlight</t>
   </si>
   <si>
@@ -172,16 +172,16 @@
     <t>http://www.baidu.com</t>
   </si>
   <si>
-    <t>TC001功能测试</t>
+    <t>TC002功能测试</t>
   </si>
   <si>
     <t>百度搜索</t>
   </si>
   <si>
-    <t>TC001性能测试</t>
-  </si>
-  <si>
-    <t>TC002自动化测试</t>
+    <t>TC002性能测试</t>
+  </si>
+  <si>
+    <t>TC003自动化测试</t>
   </si>
   <si>
     <t>TCID</t>
@@ -634,10 +634,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -678,11 +678,42 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -691,7 +722,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -705,14 +736,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -749,14 +773,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -772,6 +788,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -780,16 +804,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -798,22 +814,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -846,13 +846,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -864,25 +858,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,19 +888,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -924,13 +906,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -948,24 +930,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -978,7 +942,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,31 +996,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1026,7 +1026,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1057,9 +1057,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1075,6 +1077,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1141,152 +1152,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1761,7 +1761,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -2081,7 +2081,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="5"/>
@@ -2090,7 +2090,7 @@
     <col min="2" max="2" width="7.85714285714286" style="12" customWidth="1"/>
     <col min="3" max="3" width="11.7238095238095" style="12" customWidth="1"/>
     <col min="4" max="4" width="19.4285714285714" style="12" customWidth="1"/>
-    <col min="5" max="5" width="34" style="12" customWidth="1"/>
+    <col min="5" max="5" width="12.5714285714286" style="12" customWidth="1"/>
     <col min="6" max="1024" width="9" style="12"/>
   </cols>
   <sheetData>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:6">
       <c r="A2" s="19" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" s="19">
         <v>1</v>
@@ -2128,7 +2128,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>7</v>
@@ -2136,7 +2136,7 @@
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:6">
       <c r="A3" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="19">
         <v>1</v>
@@ -2145,18 +2145,16 @@
         <v>18</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="19" t="s">
         <v>20</v>
       </c>
+      <c r="E3" s="19"/>
       <c r="F3" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:6">
       <c r="A4" s="19" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B4" s="19">
         <v>1</v>
@@ -2165,11 +2163,9 @@
         <v>18</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>12</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E4" s="19"/>
       <c r="F4" s="19" t="s">
         <v>7</v>
       </c>
@@ -2186,8 +2182,8 @@
   <sheetPr/>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="5"/>
@@ -2199,7 +2195,8 @@
     <col min="5" max="5" width="17" style="20" customWidth="1"/>
     <col min="6" max="6" width="9.28571428571429" style="20" customWidth="1"/>
     <col min="7" max="7" width="11.2857142857143" style="20" customWidth="1"/>
-    <col min="8" max="1024" width="9" style="12"/>
+    <col min="8" max="1023" width="9" style="12"/>
+    <col min="1024" max="1024" width="9"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:9">
@@ -2210,13 +2207,13 @@
         <v>16</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>17</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>24</v>
@@ -2236,7 +2233,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13" t="s">
@@ -2257,7 +2254,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>29</v>
@@ -2282,7 +2279,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>32</v>
@@ -2309,7 +2306,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13" t="s">
@@ -2330,7 +2327,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
@@ -2378,7 +2375,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>37</v>
@@ -2427,8 +2424,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.98095238095238" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2447,7 +2444,7 @@
         <v>43</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>44</v>
@@ -2745,7 +2742,7 @@
     </row>
     <row r="4" ht="31.5" customHeight="1" spans="1:15">
       <c r="A4" s="13" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>6</v>
@@ -2790,7 +2787,7 @@
     </row>
     <row r="5" ht="15.75" spans="1:15">
       <c r="A5" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>74</v>
@@ -2837,7 +2834,7 @@
     </row>
     <row r="6" ht="47.25" spans="1:15">
       <c r="A6" s="13" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
optimize the ui actions
</commit_message>
<xml_diff>
--- a/test_cases/e2e_test_cases.xlsx
+++ b/test_cases/e2e_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="850" activeTab="5"/>
+    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -699,9 +699,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
@@ -743,6 +743,11 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -750,28 +755,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -786,7 +771,31 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -808,6 +817,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -826,14 +849,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -854,31 +870,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -922,91 +922,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,7 +958,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1036,13 +1030,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1054,55 +1096,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1127,6 +1127,17 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1179,11 +1190,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1203,166 +1220,149 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2917,8 +2917,8 @@
   <sheetPr/>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="5"/>
@@ -3341,7 +3341,7 @@
   <sheetPr/>
   <dimension ref="A1:AMD9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
optimize the ui verify actions
</commit_message>
<xml_diff>
--- a/test_cases/e2e_test_cases.xlsx
+++ b/test_cases/e2e_test_cases.xlsx
@@ -700,8 +700,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
@@ -743,6 +743,20 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -755,24 +769,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -787,45 +832,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -849,22 +864,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -878,7 +878,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -890,12 +890,12 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -922,13 +922,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -940,31 +994,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -976,19 +1006,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1000,49 +1030,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,49 +1054,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1127,41 +1127,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1191,21 +1156,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1228,141 +1178,191 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>

<commit_message>
updated end to end suite creation
</commit_message>
<xml_diff>
--- a/test_cases/e2e_test_cases.xlsx
+++ b/test_cases/e2e_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="850" activeTab="11"/>
+    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="850" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,10 @@
     <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
-    <definedName name="Endpoint">api_test_cases.xlsx!Table5[Run]</definedName>
-    <definedName name="Header">api_test_cases.xlsx!Table4[#Data]</definedName>
-    <definedName name="BodyTemplate">api_test_cases.xlsx!Endpoints[Environment]</definedName>
-    <definedName name="BodyDefault">api_test_cases.xlsx!Table1[#Data]</definedName>
+    <definedName name="Endpoint">'C:\Users\vhuang1\PycharmProjects\api_test_framework\test_cases\api_test_cases.xlsx'!Table5[Run]</definedName>
+    <definedName name="Header">'C:\Users\vhuang1\PycharmProjects\api_test_framework\test_cases\api_test_cases.xlsx'!Table4[#Data]</definedName>
+    <definedName name="BodyTemplate">'C:\Users\vhuang1\PycharmProjects\api_test_framework\test_cases\api_test_cases.xlsx'!Endpoints[Environment]</definedName>
+    <definedName name="BodyDefault">'C:\Users\vhuang1\PycharmProjects\api_test_framework\test_cases\api_test_cases.xlsx'!Table1[#Data]</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="164">
   <si>
     <t>Run</t>
   </si>
@@ -91,6 +91,15 @@
     <t>API_pacs008</t>
   </si>
   <si>
+    <t>Baidu_Search3</t>
+  </si>
+  <si>
+    <t>insert data</t>
+  </si>
+  <si>
+    <t>tag1</t>
+  </si>
+  <si>
     <t>OB_pacs008_1</t>
   </si>
   <si>
@@ -100,9 +109,6 @@
     <t>tag1,sanity check</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Baidu_Search</t>
   </si>
   <si>
@@ -112,19 +118,10 @@
     <t>Search for software testing</t>
   </si>
   <si>
-    <t>tag1</t>
-  </si>
-  <si>
     <t>Baidu_Search2</t>
   </si>
   <si>
     <t>Search for frontend development</t>
-  </si>
-  <si>
-    <t>Baidu_Search3</t>
-  </si>
-  <si>
-    <t>insert data</t>
   </si>
   <si>
     <t>Step ID</t>
@@ -306,6 +303,9 @@
     <t>Body Default</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>Position</t>
   </si>
   <si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>j_pacs.008_in</t>
+  </si>
+  <si>
+    <t>pacs0082</t>
   </si>
   <si>
     <t xml:space="preserve">Executes an outbound credit transfer (pacs008 out cny 100) of 100 CNY. </t>
@@ -637,7 +640,7 @@
   "disable-dev-shm-usage": true,
   "disable-gpu": true,
   "remote-debugging-port": 9222,
-  "headless": false
+  "headless": true
 }</t>
   </si>
   <si>
@@ -747,8 +750,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -791,9 +794,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -803,8 +808,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -819,14 +829,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -845,6 +848,20 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -887,8 +904,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -896,7 +914,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -910,23 +928,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -970,19 +973,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -994,19 +1021,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1018,19 +1051,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1048,61 +1105,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1114,31 +1123,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1151,6 +1136,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1175,21 +1178,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1219,6 +1207,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1238,15 +1241,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1276,141 +1270,150 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2542,7 +2545,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99047619047619" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -2580,7 +2583,7 @@
       <c r="B2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="17" t="s">
@@ -2590,55 +2593,55 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:5">
+    <row r="3" ht="15.75" spans="1:5">
       <c r="A3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:5">
       <c r="A4" s="17" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>16</v>
-      </c>
       <c r="E4" s="17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="5" ht="15.75" spans="1:5">
+    <row r="5" ht="15.75" customHeight="1" spans="1:5">
       <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>18</v>
-      </c>
       <c r="E5" s="17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2666,10 +2669,10 @@
   <sheetData>
     <row r="1" s="8" customFormat="1" ht="15.75" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" s="8" customFormat="1" ht="201" customHeight="1" spans="1:2">
@@ -2677,15 +2680,15 @@
         <v>91</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" s="8" customFormat="1" ht="201" customHeight="1" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2703,7 +2706,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.11428571428571" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -2722,92 +2725,92 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.75" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="120" spans="1:10">
       <c r="A2" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="120" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C3" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2825,8 +2828,8 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.11428571428571" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -2839,35 +2842,35 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.75" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2900,35 +2903,35 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.75" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="60" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="75" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2965,16 +2968,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:6">
@@ -2982,19 +2985,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="17">
         <v>1</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:6">
@@ -3002,16 +3005,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="17">
         <v>1</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="17"/>
     </row>
@@ -3020,16 +3023,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="17">
         <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="17"/>
     </row>
@@ -3038,16 +3041,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C5" s="17">
         <v>1</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="17"/>
     </row>
@@ -3086,28 +3089,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:9">
@@ -3115,17 +3118,17 @@
         <v>5</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>35</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="15"/>
@@ -3136,19 +3139,19 @@
         <v>5</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>38</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>5</v>
@@ -3161,16 +3164,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>40</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="15" t="s">
@@ -3188,17 +3191,17 @@
         <v>5</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>41</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>42</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="15"/>
@@ -3209,14 +3212,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -3228,17 +3231,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>44</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>45</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="15"/>
@@ -3275,44 +3278,44 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4">
       <c r="A2" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>48</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4">
       <c r="A3" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3345,198 +3348,198 @@
         <v>2</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>53</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:5">
       <c r="A2" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:5">
       <c r="A3" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:5">
       <c r="A4" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:5">
       <c r="A5" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="13">
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:5">
       <c r="A6" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="13">
         <v>2</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:5">
       <c r="A7" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="13">
         <v>2</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:5">
       <c r="A8" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:5">
       <c r="A9" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="1:5">
       <c r="A10" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:5">
       <c r="A11" s="17" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:5">
       <c r="A12" s="17" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B12" s="13">
         <v>1</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" ht="76.5" spans="1:5">
       <c r="A13" s="17" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="E13" s="19" t="s">
         <v>65</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3551,8 +3554,8 @@
   <sheetPr/>
   <dimension ref="A1:AMD9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
@@ -3585,48 +3588,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" ht="16.5" customHeight="1" spans="1:15">
       <c r="A2" s="13" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13" t="s">
@@ -3655,7 +3658,7 @@
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:15">
       <c r="A3" s="13" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
@@ -3725,7 +3728,7 @@
         <v>91</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="O4" s="15"/>
     </row>
@@ -3734,43 +3737,43 @@
         <v>5</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G5" s="13">
         <v>200</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="O5" s="15">
         <v>1</v>
@@ -3781,16 +3784,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>87</v>
@@ -3799,10 +3802,10 @@
         <v>200</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>90</v>
@@ -3817,7 +3820,7 @@
         <v>91</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="O6" s="15"/>
     </row>
@@ -6926,142 +6929,142 @@
   <sheetData>
     <row r="1" s="8" customFormat="1" ht="15.75" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" s="8" customFormat="1" spans="1:4">
       <c r="A2" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" s="8" customFormat="1" spans="1:4">
       <c r="A3" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" s="8" customFormat="1" spans="1:4">
       <c r="A4" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" s="8" customFormat="1" spans="1:4">
       <c r="A5" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>90</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" s="8" customFormat="1" spans="1:4">
       <c r="A6" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" s="8" customFormat="1" spans="1:4">
       <c r="A7" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>79</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" s="8" customFormat="1" spans="1:4">
       <c r="A8" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>90</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" s="8" customFormat="1" spans="1:4">
       <c r="A9" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" s="8" customFormat="1" spans="1:4">
       <c r="A10" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>79</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -7102,10 +7105,10 @@
   <sheetData>
     <row r="1" s="8" customFormat="1" ht="15.75" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" s="8" customFormat="1" ht="120" spans="1:2">
@@ -7113,15 +7116,15 @@
         <v>80</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" s="8" customFormat="1" ht="60" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -7151,13 +7154,13 @@
   <sheetData>
     <row r="1" s="8" customFormat="1" ht="15.75" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" s="8" customFormat="1" ht="201" customHeight="1" spans="1:3">
@@ -7165,21 +7168,21 @@
         <v>91</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" s="8" customFormat="1" ht="201" customHeight="1" spans="1:3">
       <c r="A3" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>